<commit_message>
Chile coordinates + fix of csv delimiter
csv delimiter was ; for some reason
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eica\covid\covid-19_latinoamerica\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanHP\Desktop\GitHub\covid-19_pe\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC82C6-E00A-4B17-A7CD-36EBAF6BD3F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="14445" windowHeight="8250"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso3312" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="818">
   <si>
     <t>Country Code</t>
   </si>
@@ -2478,7 +2479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3278,10 +3279,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4954,8 +4957,17 @@
       <c r="D88" t="s">
         <v>237</v>
       </c>
+      <c r="E88" t="s">
+        <v>21</v>
+      </c>
       <c r="F88" t="s">
         <v>238</v>
+      </c>
+      <c r="G88">
+        <v>-46.035339</v>
+      </c>
+      <c r="H88">
+        <v>-73.036434999999997</v>
       </c>
       <c r="L88" t="s">
         <v>239</v>
@@ -4974,8 +4986,17 @@
       <c r="D89" t="s">
         <v>241</v>
       </c>
+      <c r="E89" t="s">
+        <v>21</v>
+      </c>
       <c r="F89" t="s">
         <v>242</v>
+      </c>
+      <c r="G89">
+        <v>-23.446308999999999</v>
+      </c>
+      <c r="H89">
+        <v>-68.998489000000006</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -4991,8 +5012,17 @@
       <c r="D90" t="s">
         <v>244</v>
       </c>
+      <c r="E90" t="s">
+        <v>21</v>
+      </c>
       <c r="F90" t="s">
         <v>245</v>
+      </c>
+      <c r="G90">
+        <v>-18.539467999999999</v>
+      </c>
+      <c r="H90">
+        <v>-69.714607999999998</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -5008,8 +5038,17 @@
       <c r="D91" t="s">
         <v>247</v>
       </c>
+      <c r="E91" t="s">
+        <v>21</v>
+      </c>
       <c r="F91" t="s">
         <v>248</v>
+      </c>
+      <c r="G91">
+        <v>-38.782228000000003</v>
+      </c>
+      <c r="H91">
+        <v>-72.543251999999995</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -5025,8 +5064,17 @@
       <c r="D92" t="s">
         <v>250</v>
       </c>
+      <c r="E92" t="s">
+        <v>21</v>
+      </c>
       <c r="F92" t="s">
         <v>251</v>
+      </c>
+      <c r="G92">
+        <v>-27.648325</v>
+      </c>
+      <c r="H92">
+        <v>-70.432531999999995</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -5042,8 +5090,17 @@
       <c r="D93" t="s">
         <v>253</v>
       </c>
+      <c r="E93" t="s">
+        <v>21</v>
+      </c>
       <c r="F93" t="s">
         <v>254</v>
+      </c>
+      <c r="G93">
+        <v>-37.225611999999998</v>
+      </c>
+      <c r="H93">
+        <v>-73.108534000000006</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -5059,8 +5116,17 @@
       <c r="D94" t="s">
         <v>256</v>
       </c>
+      <c r="E94" t="s">
+        <v>21</v>
+      </c>
       <c r="F94" t="s">
         <v>257</v>
+      </c>
+      <c r="G94">
+        <v>-30.540376999999999</v>
+      </c>
+      <c r="H94">
+        <v>-70.967738999999995</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -5076,8 +5142,17 @@
       <c r="D95" t="s">
         <v>259</v>
       </c>
+      <c r="E95" t="s">
+        <v>21</v>
+      </c>
       <c r="F95" t="s">
         <v>260</v>
+      </c>
+      <c r="G95">
+        <v>-34.434587999999998</v>
+      </c>
+      <c r="H95">
+        <v>-71.154459000000003</v>
       </c>
       <c r="L95" t="s">
         <v>261</v>
@@ -5096,8 +5171,17 @@
       <c r="D96" t="s">
         <v>263</v>
       </c>
+      <c r="E96" t="s">
+        <v>21</v>
+      </c>
       <c r="F96" t="s">
         <v>264</v>
+      </c>
+      <c r="G96">
+        <v>-42.046638000000002</v>
+      </c>
+      <c r="H96">
+        <v>-73.008763999999999</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -5113,8 +5197,17 @@
       <c r="D97" t="s">
         <v>266</v>
       </c>
+      <c r="E97" t="s">
+        <v>21</v>
+      </c>
       <c r="F97" t="s">
         <v>267</v>
+      </c>
+      <c r="G97">
+        <v>-39.922539</v>
+      </c>
+      <c r="H97">
+        <v>-72.588984999999994</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -5130,8 +5223,17 @@
       <c r="D98" t="s">
         <v>269</v>
       </c>
+      <c r="E98" t="s">
+        <v>21</v>
+      </c>
       <c r="F98" t="s">
         <v>270</v>
+      </c>
+      <c r="G98">
+        <v>-51.902416000000002</v>
+      </c>
+      <c r="H98">
+        <v>-73.244017999999997</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -5147,8 +5249,17 @@
       <c r="D99" t="s">
         <v>272</v>
       </c>
+      <c r="E99" t="s">
+        <v>21</v>
+      </c>
       <c r="F99" t="s">
         <v>273</v>
+      </c>
+      <c r="G99">
+        <v>-35.500971999999997</v>
+      </c>
+      <c r="H99">
+        <v>-71.727129000000005</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -5164,6 +5275,15 @@
       <c r="D100" t="s">
         <v>275</v>
       </c>
+      <c r="E100" t="s">
+        <v>21</v>
+      </c>
+      <c r="G100">
+        <v>-36.602809999999998</v>
+      </c>
+      <c r="H100">
+        <v>-72.073119000000005</v>
+      </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -5178,8 +5298,17 @@
       <c r="D101" t="s">
         <v>277</v>
       </c>
+      <c r="E101" t="s">
+        <v>21</v>
+      </c>
       <c r="F101" t="s">
         <v>278</v>
+      </c>
+      <c r="G101">
+        <v>-33.478729000000001</v>
+      </c>
+      <c r="H101">
+        <v>-70.590025999999995</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -5195,8 +5324,17 @@
       <c r="D102" t="s">
         <v>280</v>
       </c>
+      <c r="E102" t="s">
+        <v>21</v>
+      </c>
       <c r="F102" t="s">
         <v>281</v>
+      </c>
+      <c r="G102">
+        <v>-20.099081000000002</v>
+      </c>
+      <c r="H102">
+        <v>-69.456920999999994</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -5212,8 +5350,17 @@
       <c r="D103" t="s">
         <v>283</v>
       </c>
+      <c r="E103" t="s">
+        <v>21</v>
+      </c>
       <c r="F103" t="s">
         <v>284</v>
+      </c>
+      <c r="G103">
+        <v>-32.740869000000004</v>
+      </c>
+      <c r="H103">
+        <v>-71.404539</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ISO 3166-2 up to 2020-03-23 & format
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -12,9 +12,12 @@
     <workbookView xWindow="840" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="iso3312" sheetId="1" r:id="rId1"/>
+    <sheet name="iso3312_latinamerica" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">iso3312_latinamerica!$A$1:$L$355</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -3281,11 +3284,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3333,19 +3341,25 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>-77.107550000000003</v>
+      </c>
+      <c r="H2">
+        <v>-11.82297</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3356,19 +3370,25 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
+      <c r="G3">
+        <v>-9.5274999999999999</v>
+      </c>
+      <c r="H3">
+        <v>-77.533299999999997</v>
+      </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3379,19 +3399,25 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
+      <c r="G4">
+        <v>-73</v>
+      </c>
+      <c r="H4">
+        <v>-14</v>
+      </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3402,19 +3428,25 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
+      <c r="G5">
+        <v>-16.398889499999999</v>
+      </c>
+      <c r="H5">
+        <v>-71.535003700000004</v>
+      </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3425,19 +3457,25 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
+      <c r="G6">
+        <v>-13.1587801</v>
+      </c>
+      <c r="H6">
+        <v>-74.223213200000004</v>
+      </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3448,19 +3486,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
+      <c r="G7">
+        <v>-7.15639</v>
+      </c>
+      <c r="H7">
+        <v>-78.515600000000006</v>
+      </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3471,19 +3515,25 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
+      <c r="G8">
+        <v>-13.5226402</v>
+      </c>
+      <c r="H8">
+        <v>-71.967338600000005</v>
+      </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3494,19 +3544,25 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
+      <c r="G9">
+        <v>-12.0542</v>
+      </c>
+      <c r="H9">
+        <v>-77.128900000000002</v>
+      </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3517,19 +3573,25 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
+      <c r="G10">
+        <v>-12.786899999999999</v>
+      </c>
+      <c r="H10">
+        <v>-74.973100000000002</v>
+      </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3540,19 +3602,25 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
+      <c r="G11">
+        <v>-9.9306201999999999</v>
+      </c>
+      <c r="H11">
+        <v>-76.242233299999995</v>
+      </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3563,19 +3631,25 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
       </c>
+      <c r="G12">
+        <v>-14.067769999999999</v>
+      </c>
+      <c r="H12">
+        <v>-75.728607199999999</v>
+      </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3586,19 +3660,25 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
       </c>
+      <c r="G13">
+        <v>-76.011920000000003</v>
+      </c>
+      <c r="H13">
+        <v>-11.18881</v>
+      </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3609,19 +3689,25 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
+      <c r="G14">
+        <v>-8.1159897000000001</v>
+      </c>
+      <c r="H14">
+        <v>-79.0299835</v>
+      </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3632,19 +3718,25 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
       </c>
+      <c r="G15">
+        <v>-79.932839999999999</v>
+      </c>
+      <c r="H15">
+        <v>-6.67387</v>
+      </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3655,19 +3747,25 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
       </c>
+      <c r="G16">
+        <v>-12.0431805</v>
+      </c>
+      <c r="H16">
+        <v>-77.028236399999997</v>
+      </c>
       <c r="I16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3678,19 +3776,25 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
+      <c r="G17">
+        <v>-3.74912</v>
+      </c>
+      <c r="H17">
+        <v>-73.253829999999994</v>
+      </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3701,19 +3805,25 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
+      <c r="G18">
+        <v>-12.5933104</v>
+      </c>
+      <c r="H18">
+        <v>-69.189132700000002</v>
+      </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3724,19 +3834,25 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
+      <c r="G19">
+        <v>-70.935670000000002</v>
+      </c>
+      <c r="H19">
+        <v>-17.198319999999999</v>
+      </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3747,19 +3863,25 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>-12.0431805</v>
+      </c>
+      <c r="H20">
+        <v>-77.028236399999997</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3778,6 +3900,12 @@
       <c r="E21" t="s">
         <v>21</v>
       </c>
+      <c r="G21">
+        <v>-10.6674805</v>
+      </c>
+      <c r="H21">
+        <v>-76.256683300000006</v>
+      </c>
       <c r="I21" t="s">
         <v>85</v>
       </c>
@@ -3801,6 +3929,12 @@
       <c r="E22" t="s">
         <v>21</v>
       </c>
+      <c r="G22">
+        <v>-5.1972199999999997</v>
+      </c>
+      <c r="H22">
+        <v>-80.6267</v>
+      </c>
       <c r="I22" t="s">
         <v>88</v>
       </c>
@@ -3824,6 +3958,12 @@
       <c r="E23" t="s">
         <v>21</v>
       </c>
+      <c r="G23">
+        <v>-70.019900000000007</v>
+      </c>
+      <c r="H23">
+        <v>-15.8422</v>
+      </c>
       <c r="I23" t="s">
         <v>91</v>
       </c>
@@ -3847,6 +3987,12 @@
       <c r="E24" t="s">
         <v>21</v>
       </c>
+      <c r="G24">
+        <v>-12.0303</v>
+      </c>
+      <c r="H24">
+        <v>-77.057199999999995</v>
+      </c>
       <c r="I24" t="s">
         <v>94</v>
       </c>
@@ -3870,6 +4016,12 @@
       <c r="E25" t="s">
         <v>21</v>
       </c>
+      <c r="G25">
+        <v>-70.253619999999998</v>
+      </c>
+      <c r="H25">
+        <v>-18.01465</v>
+      </c>
       <c r="I25" t="s">
         <v>97</v>
       </c>
@@ -3893,6 +4045,12 @@
       <c r="E26" t="s">
         <v>21</v>
       </c>
+      <c r="G26">
+        <v>-3.5669401000000001</v>
+      </c>
+      <c r="H26">
+        <v>-80.451530500000004</v>
+      </c>
       <c r="I26" t="s">
         <v>101</v>
       </c>
@@ -3916,6 +4074,12 @@
       <c r="E27" t="s">
         <v>21</v>
       </c>
+      <c r="G27">
+        <v>-8.3791504000000003</v>
+      </c>
+      <c r="H27">
+        <v>-74.553871200000003</v>
+      </c>
       <c r="I27" t="s">
         <v>104</v>
       </c>
@@ -7470,6 +7634,12 @@
       <c r="E232" t="s">
         <v>562</v>
       </c>
+      <c r="G232">
+        <v>19.441647</v>
+      </c>
+      <c r="H232">
+        <v>-99.151883999999995</v>
+      </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
@@ -7487,6 +7657,12 @@
       <c r="E233" t="s">
         <v>181</v>
       </c>
+      <c r="G233">
+        <v>21.879822999999998</v>
+      </c>
+      <c r="H233">
+        <v>-102.296047</v>
+      </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
@@ -7504,6 +7680,12 @@
       <c r="E234" t="s">
         <v>181</v>
       </c>
+      <c r="G234">
+        <v>32.641176000000002</v>
+      </c>
+      <c r="H234">
+        <v>-115.475579</v>
+      </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
@@ -7521,6 +7703,12 @@
       <c r="E235" t="s">
         <v>181</v>
       </c>
+      <c r="G235">
+        <v>24.148745000000002</v>
+      </c>
+      <c r="H235">
+        <v>-110.30659</v>
+      </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
@@ -7538,6 +7726,12 @@
       <c r="E236" t="s">
         <v>181</v>
       </c>
+      <c r="G236">
+        <v>19.844814</v>
+      </c>
+      <c r="H236">
+        <v>-90.539648999999997</v>
+      </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
@@ -7555,6 +7749,12 @@
       <c r="E237" t="s">
         <v>181</v>
       </c>
+      <c r="G237">
+        <v>19.844814</v>
+      </c>
+      <c r="H237">
+        <v>-90.539648999999997</v>
+      </c>
       <c r="L237" t="s">
         <v>573</v>
       </c>
@@ -7575,6 +7775,12 @@
       <c r="E238" t="s">
         <v>181</v>
       </c>
+      <c r="G238">
+        <v>19.242922</v>
+      </c>
+      <c r="H238">
+        <v>-103.72811900000001</v>
+      </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
@@ -7592,6 +7798,12 @@
       <c r="E239" t="s">
         <v>181</v>
       </c>
+      <c r="G239">
+        <v>16.753972000000001</v>
+      </c>
+      <c r="H239">
+        <v>-93.115191999999993</v>
+      </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
@@ -7609,6 +7821,12 @@
       <c r="E240" t="s">
         <v>181</v>
       </c>
+      <c r="G240">
+        <v>28.636793999999998</v>
+      </c>
+      <c r="H240">
+        <v>-106.076307</v>
+      </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
@@ -7626,6 +7844,12 @@
       <c r="E241" t="s">
         <v>181</v>
       </c>
+      <c r="G241">
+        <v>24.023987999999999</v>
+      </c>
+      <c r="H241">
+        <v>-104.670194</v>
+      </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
@@ -7643,6 +7867,12 @@
       <c r="E242" t="s">
         <v>181</v>
       </c>
+      <c r="G242">
+        <v>21.016098</v>
+      </c>
+      <c r="H242">
+        <v>-101.253621</v>
+      </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
@@ -7660,6 +7890,12 @@
       <c r="E243" t="s">
         <v>181</v>
       </c>
+      <c r="G243">
+        <v>17.551649000000001</v>
+      </c>
+      <c r="H243">
+        <v>-99.501063000000002</v>
+      </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
@@ -7677,6 +7913,12 @@
       <c r="E244" t="s">
         <v>181</v>
       </c>
+      <c r="G244">
+        <v>20.12236</v>
+      </c>
+      <c r="H244">
+        <v>-98.737001000000006</v>
+      </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
@@ -7694,6 +7936,12 @@
       <c r="E245" t="s">
         <v>181</v>
       </c>
+      <c r="G245">
+        <v>20.676389</v>
+      </c>
+      <c r="H245">
+        <v>-103.34222200000001</v>
+      </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
@@ -7711,6 +7959,12 @@
       <c r="E246" t="s">
         <v>181</v>
       </c>
+      <c r="G246">
+        <v>19.293488</v>
+      </c>
+      <c r="H246">
+        <v>-99.657317000000006</v>
+      </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
@@ -7728,6 +7982,12 @@
       <c r="E247" t="s">
         <v>181</v>
       </c>
+      <c r="G247">
+        <v>19.703384</v>
+      </c>
+      <c r="H247">
+        <v>-101.192046</v>
+      </c>
       <c r="L247" t="s">
         <v>594</v>
       </c>
@@ -7748,6 +8008,12 @@
       <c r="E248" t="s">
         <v>181</v>
       </c>
+      <c r="G248">
+        <v>18.921783000000001</v>
+      </c>
+      <c r="H248">
+        <v>-99.234897000000004</v>
+      </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
@@ -7765,6 +8031,12 @@
       <c r="E249" t="s">
         <v>181</v>
       </c>
+      <c r="G249">
+        <v>21.507413</v>
+      </c>
+      <c r="H249">
+        <v>-104.893799</v>
+      </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
@@ -7782,6 +8054,12 @@
       <c r="E250" t="s">
         <v>181</v>
       </c>
+      <c r="G250">
+        <v>25.664697</v>
+      </c>
+      <c r="H250">
+        <v>-100.310892</v>
+      </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
@@ -7799,6 +8077,12 @@
       <c r="E251" t="s">
         <v>181</v>
       </c>
+      <c r="G251">
+        <v>17.059992999999999</v>
+      </c>
+      <c r="H251">
+        <v>-96.725449999999995</v>
+      </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
@@ -7816,6 +8100,12 @@
       <c r="E252" t="s">
         <v>181</v>
       </c>
+      <c r="G252">
+        <v>19.043990000000001</v>
+      </c>
+      <c r="H252">
+        <v>-98.197495000000004</v>
+      </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
@@ -7833,6 +8123,12 @@
       <c r="E253" t="s">
         <v>181</v>
       </c>
+      <c r="G253">
+        <v>20.593391</v>
+      </c>
+      <c r="H253">
+        <v>-100.389957</v>
+      </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
@@ -7850,6 +8146,12 @@
       <c r="E254" t="s">
         <v>181</v>
       </c>
+      <c r="G254">
+        <v>18.493888999999999</v>
+      </c>
+      <c r="H254">
+        <v>-88.297899000000001</v>
+      </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
@@ -7867,6 +8169,12 @@
       <c r="E255" t="s">
         <v>181</v>
       </c>
+      <c r="G255">
+        <v>22.151655000000002</v>
+      </c>
+      <c r="H255">
+        <v>-100.976958</v>
+      </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
@@ -7884,6 +8192,12 @@
       <c r="E256" t="s">
         <v>181</v>
       </c>
+      <c r="G256">
+        <v>24.808807999999999</v>
+      </c>
+      <c r="H256">
+        <v>-107.393756</v>
+      </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
@@ -7901,6 +8215,12 @@
       <c r="E257" t="s">
         <v>181</v>
       </c>
+      <c r="G257">
+        <v>29.074891999999998</v>
+      </c>
+      <c r="H257">
+        <v>-110.95846400000001</v>
+      </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
@@ -7918,6 +8238,12 @@
       <c r="E258" t="s">
         <v>181</v>
       </c>
+      <c r="G258">
+        <v>17.987838</v>
+      </c>
+      <c r="H258">
+        <v>-92.919415999999998</v>
+      </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -7935,6 +8261,12 @@
       <c r="E259" t="s">
         <v>181</v>
       </c>
+      <c r="G259">
+        <v>23.731052999999999</v>
+      </c>
+      <c r="H259">
+        <v>-99.151250000000005</v>
+      </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
@@ -7952,6 +8284,12 @@
       <c r="E260" t="s">
         <v>181</v>
       </c>
+      <c r="G260">
+        <v>19.316552999999999</v>
+      </c>
+      <c r="H260">
+        <v>-98.237639999999999</v>
+      </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
@@ -7969,6 +8307,12 @@
       <c r="E261" t="s">
         <v>181</v>
       </c>
+      <c r="G261">
+        <v>19.527085</v>
+      </c>
+      <c r="H261">
+        <v>-96.922645000000003</v>
+      </c>
       <c r="L261" t="s">
         <v>623</v>
       </c>
@@ -7989,6 +8333,12 @@
       <c r="E262" t="s">
         <v>181</v>
       </c>
+      <c r="G262">
+        <v>20.967537</v>
+      </c>
+      <c r="H262">
+        <v>-89.624392</v>
+      </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
@@ -8006,6 +8356,12 @@
       <c r="E263" t="s">
         <v>181</v>
       </c>
+      <c r="G263">
+        <v>22.776095999999999</v>
+      </c>
+      <c r="H263">
+        <v>-102.571836</v>
+      </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
@@ -8949,7 +9305,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>730</v>
       </c>
@@ -8963,7 +9319,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>730</v>
       </c>
@@ -8977,7 +9333,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>730</v>
       </c>
@@ -8991,7 +9347,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>730</v>
       </c>
@@ -9005,7 +9361,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>730</v>
       </c>
@@ -9019,7 +9375,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>730</v>
       </c>
@@ -9033,7 +9389,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>730</v>
       </c>
@@ -9047,7 +9403,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>730</v>
       </c>
@@ -9061,7 +9417,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>730</v>
       </c>
@@ -9075,7 +9431,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>730</v>
       </c>
@@ -9089,7 +9445,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>768</v>
       </c>
@@ -9105,8 +9461,14 @@
       <c r="E331" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G331">
+        <v>10.4880104</v>
+      </c>
+      <c r="H331">
+        <v>-66.879188499999998</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>768</v>
       </c>
@@ -9123,7 +9485,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>768</v>
       </c>
@@ -9139,8 +9501,14 @@
       <c r="E333" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G333">
+        <v>5.6604900000000002</v>
+      </c>
+      <c r="H333">
+        <v>-67.583427400000005</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>768</v>
       </c>
@@ -9156,8 +9524,14 @@
       <c r="E334" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G334">
+        <v>10.216670000000001</v>
+      </c>
+      <c r="H334">
+        <v>-64.616668700000005</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>768</v>
       </c>
@@ -9173,8 +9547,14 @@
       <c r="E335" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G335">
+        <v>7.8878197999999999</v>
+      </c>
+      <c r="H335">
+        <v>-67.472358700000001</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>768</v>
       </c>
@@ -9190,8 +9570,14 @@
       <c r="E336" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G336">
+        <v>10.2353497</v>
+      </c>
+      <c r="H336">
+        <v>-67.591133099999993</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>768</v>
       </c>
@@ -9207,8 +9593,14 @@
       <c r="E337" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G337">
+        <v>8.6226100999999993</v>
+      </c>
+      <c r="H337">
+        <v>-70.207488999999995</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>768</v>
       </c>
@@ -9224,8 +9616,14 @@
       <c r="E338" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G338">
+        <v>8.1292294999999992</v>
+      </c>
+      <c r="H338">
+        <v>-63.5408592</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>768</v>
       </c>
@@ -9241,8 +9639,14 @@
       <c r="E339" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G339">
+        <v>10.1620197</v>
+      </c>
+      <c r="H339">
+        <v>-68.007652300000004</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>768</v>
       </c>
@@ -9258,8 +9662,14 @@
       <c r="E340" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G340">
+        <v>9.6612396</v>
+      </c>
+      <c r="H340">
+        <v>-68.5826797</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>768</v>
       </c>
@@ -9275,8 +9685,14 @@
       <c r="E341" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G341">
+        <v>9.0580596999999994</v>
+      </c>
+      <c r="H341">
+        <v>-62.049999200000002</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>768</v>
       </c>
@@ -9292,8 +9708,14 @@
       <c r="E342" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G342">
+        <v>11.6955996</v>
+      </c>
+      <c r="H342">
+        <v>-70.199569699999998</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>768</v>
       </c>
@@ -9309,8 +9731,14 @@
       <c r="E343" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G343">
+        <v>9.9115199999999994</v>
+      </c>
+      <c r="H343">
+        <v>-67.353813200000005</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>768</v>
       </c>
@@ -9326,8 +9754,14 @@
       <c r="E344" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G344">
+        <v>10.0647001</v>
+      </c>
+      <c r="H344">
+        <v>-69.357032799999999</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>768</v>
       </c>
@@ -9343,8 +9777,14 @@
       <c r="E345" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G345">
+        <v>8.5897197999999992</v>
+      </c>
+      <c r="H345">
+        <v>-71.156112699999994</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>768</v>
       </c>
@@ -9360,8 +9800,14 @@
       <c r="E346" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G346">
+        <v>10.472260500000001</v>
+      </c>
+      <c r="H346">
+        <v>-66.801551799999999</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>768</v>
       </c>
@@ -9377,8 +9823,14 @@
       <c r="E347" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G347">
+        <v>9.7456902999999997</v>
+      </c>
+      <c r="H347">
+        <v>-63.183231399999997</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>768</v>
       </c>
@@ -9394,8 +9846,14 @@
       <c r="E348" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G348">
+        <v>10.9577103</v>
+      </c>
+      <c r="H348">
+        <v>-63.869709</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>768</v>
       </c>
@@ -9411,8 +9869,14 @@
       <c r="E349" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G349">
+        <v>9.0418301000000003</v>
+      </c>
+      <c r="H349">
+        <v>-69.742057799999998</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>768</v>
       </c>
@@ -9428,8 +9892,14 @@
       <c r="E350" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G350">
+        <v>10.45397</v>
+      </c>
+      <c r="H350">
+        <v>-64.182563799999997</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>768</v>
       </c>
@@ -9445,8 +9915,14 @@
       <c r="E351" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G351">
+        <v>7.7669401000000002</v>
+      </c>
+      <c r="H351">
+        <v>-72.224998499999998</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>768</v>
       </c>
@@ -9462,8 +9938,14 @@
       <c r="E352" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G352">
+        <v>9.3658304000000001</v>
+      </c>
+      <c r="H352">
+        <v>-70.436943099999993</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>768</v>
       </c>
@@ -9479,8 +9961,14 @@
       <c r="E353" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G353">
+        <v>10.596209500000001</v>
+      </c>
+      <c r="H353">
+        <v>-66.954849199999998</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>768</v>
       </c>
@@ -9496,8 +9984,14 @@
       <c r="E354" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G354">
+        <v>10.3399096</v>
+      </c>
+      <c r="H354">
+        <v>-68.742469799999995</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>768</v>
       </c>
@@ -9513,8 +10007,16 @@
       <c r="E355" t="s">
         <v>181</v>
       </c>
+      <c r="G355">
+        <v>10.666629800000001</v>
+      </c>
+      <c r="H355">
+        <v>-71.612449600000005</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L355"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix encoding of georef csv, please use UTF-8
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eica\covid\covid-19_latinoamerica\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanHP\Desktop\GitHub\covid-19_pe\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F56D9B-BA72-40BA-86C9-9FF4FA486FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso3312_latinamerica" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="819">
   <si>
     <t>Country Code</t>
   </si>
@@ -2476,12 +2477,15 @@
   </si>
   <si>
     <t>San Andrés &amp; Providencia y Santa Catalina</t>
+  </si>
+  <si>
+    <t>XVI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3281,11 +3285,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5441,6 +5445,9 @@
       <c r="E100" t="s">
         <v>21</v>
       </c>
+      <c r="F100" t="s">
+        <v>818</v>
+      </c>
       <c r="G100">
         <v>-36.602809999999998</v>
       </c>
@@ -10015,7 +10022,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L355"/>
+  <autoFilter ref="A1:L355" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Perú Lat Lon for few subdivisions
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanHP\Desktop\GitHub\covid-19_pe\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eica\covid\covid-19_latinoamerica\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F56D9B-BA72-40BA-86C9-9FF4FA486FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="iso3312_latinamerica" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="821">
   <si>
     <t>Country Code</t>
   </si>
@@ -2480,12 +2479,18 @@
   </si>
   <si>
     <t>XVI</t>
+  </si>
+  <si>
+    <t> -71.5350037</t>
+  </si>
+  <si>
+    <t> -76.9716797</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3285,11 +3290,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3354,10 +3360,10 @@
         <v>21</v>
       </c>
       <c r="G2">
-        <v>-77.107550000000003</v>
+        <v>-6.2316899000000001</v>
       </c>
       <c r="H2">
-        <v>-11.82297</v>
+        <v>-77.869033799999997</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -3383,10 +3389,10 @@
         <v>21</v>
       </c>
       <c r="G3">
-        <v>-9.5274999999999999</v>
+        <v>-9.5277901000000007</v>
       </c>
       <c r="H3">
-        <v>-77.533299999999997</v>
+        <v>-77.527778600000005</v>
       </c>
       <c r="I3" t="s">
         <v>26</v>
@@ -3412,10 +3418,10 @@
         <v>21</v>
       </c>
       <c r="G4">
-        <v>-73</v>
+        <v>-13.6338902</v>
       </c>
       <c r="H4">
-        <v>-14</v>
+        <v>-72.881393399999993</v>
       </c>
       <c r="I4" t="s">
         <v>30</v>
@@ -3443,8 +3449,8 @@
       <c r="G5">
         <v>-16.398889499999999</v>
       </c>
-      <c r="H5">
-        <v>-71.535003700000004</v>
+      <c r="H5" t="s">
+        <v>819</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -3557,10 +3563,10 @@
         <v>21</v>
       </c>
       <c r="G9">
-        <v>-12.0542</v>
+        <v>-12.056590099999999</v>
       </c>
       <c r="H9">
-        <v>-77.128900000000002</v>
+        <v>-77.118141199999997</v>
       </c>
       <c r="I9" t="s">
         <v>49</v>
@@ -3644,10 +3650,10 @@
         <v>21</v>
       </c>
       <c r="G12">
-        <v>-14.067769999999999</v>
+        <v>-13.710290000000001</v>
       </c>
       <c r="H12">
-        <v>-75.728607199999999</v>
+        <v>-76.205383299999994</v>
       </c>
       <c r="I12" t="s">
         <v>60</v>
@@ -3673,10 +3679,10 @@
         <v>21</v>
       </c>
       <c r="G13">
-        <v>-76.011920000000003</v>
+        <v>-12.0651302</v>
       </c>
       <c r="H13">
-        <v>-11.18881</v>
+        <v>75.204856899999996</v>
       </c>
       <c r="I13" t="s">
         <v>63</v>
@@ -3731,10 +3737,10 @@
         <v>21</v>
       </c>
       <c r="G15">
-        <v>-79.932839999999999</v>
+        <v>-6.7011098999999996</v>
       </c>
       <c r="H15">
-        <v>-6.67387</v>
+        <v>-79.906112699999994</v>
       </c>
       <c r="I15" t="s">
         <v>70</v>
@@ -3789,10 +3795,10 @@
         <v>21</v>
       </c>
       <c r="G17">
-        <v>-3.74912</v>
+        <v>-5.9018101999999999</v>
       </c>
       <c r="H17">
-        <v>-73.253829999999994</v>
+        <v>-76.122337299999998</v>
       </c>
       <c r="I17" t="s">
         <v>75</v>
@@ -3847,10 +3853,10 @@
         <v>21</v>
       </c>
       <c r="G19">
-        <v>-70.935670000000002</v>
+        <v>-17.1983204</v>
       </c>
       <c r="H19">
-        <v>-17.198319999999999</v>
+        <v>-70.935668899999996</v>
       </c>
       <c r="I19" t="s">
         <v>81</v>
@@ -3934,10 +3940,10 @@
         <v>21</v>
       </c>
       <c r="G22">
-        <v>-5.1972199999999997</v>
+        <v>-5.1944900000000001</v>
       </c>
       <c r="H22">
-        <v>-80.6267</v>
+        <v>-80.632820100000004</v>
       </c>
       <c r="I22" t="s">
         <v>88</v>
@@ -3963,10 +3969,10 @@
         <v>21</v>
       </c>
       <c r="G23">
-        <v>-70.019900000000007</v>
+        <v>-15.8422003</v>
       </c>
       <c r="H23">
-        <v>-15.8422</v>
+        <v>-70.019897499999999</v>
       </c>
       <c r="I23" t="s">
         <v>91</v>
@@ -3992,10 +3998,10 @@
         <v>21</v>
       </c>
       <c r="G24">
-        <v>-12.0303</v>
-      </c>
-      <c r="H24">
-        <v>-77.057199999999995</v>
+        <v>-6.0341601000000002</v>
+      </c>
+      <c r="H24" t="s">
+        <v>820</v>
       </c>
       <c r="I24" t="s">
         <v>94</v>
@@ -4021,10 +4027,10 @@
         <v>21</v>
       </c>
       <c r="G25">
-        <v>-70.253619999999998</v>
+        <v>-18.0146503</v>
       </c>
       <c r="H25">
-        <v>-18.01465</v>
+        <v>-70.253616300000004</v>
       </c>
       <c r="I25" t="s">
         <v>97</v>
@@ -4091,7 +4097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -4125,7 +4131,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -4159,7 +4165,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -4193,7 +4199,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -4227,7 +4233,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -4244,7 +4250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -4261,7 +4267,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -4278,7 +4284,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -4295,7 +4301,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -4312,7 +4318,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -4329,7 +4335,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>105</v>
       </c>
@@ -4363,7 +4369,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -4380,7 +4386,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -4397,7 +4403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -4448,7 +4454,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -4465,7 +4471,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -4482,7 +4488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -4499,7 +4505,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>157</v>
       </c>
@@ -4516,7 +4522,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>157</v>
       </c>
@@ -4533,7 +4539,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>157</v>
       </c>
@@ -4550,7 +4556,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>157</v>
       </c>
@@ -4567,7 +4573,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>157</v>
       </c>
@@ -4584,7 +4590,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>157</v>
       </c>
@@ -4601,7 +4607,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>157</v>
       </c>
@@ -4618,7 +4624,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -4635,7 +4641,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -4652,7 +4658,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>177</v>
       </c>
@@ -4669,7 +4675,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>177</v>
       </c>
@@ -4686,7 +4692,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>177</v>
       </c>
@@ -4703,7 +4709,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>177</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>177</v>
       </c>
@@ -4737,7 +4743,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>177</v>
       </c>
@@ -4754,7 +4760,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>177</v>
       </c>
@@ -4771,7 +4777,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>177</v>
       </c>
@@ -4788,7 +4794,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>177</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -4822,7 +4828,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>177</v>
       </c>
@@ -4839,7 +4845,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>177</v>
       </c>
@@ -4856,7 +4862,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -4873,7 +4879,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>177</v>
       </c>
@@ -4890,7 +4896,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>177</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>177</v>
       </c>
@@ -4924,7 +4930,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>177</v>
       </c>
@@ -4941,7 +4947,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -4958,7 +4964,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -4975,7 +4981,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -4992,7 +4998,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>177</v>
       </c>
@@ -5009,7 +5015,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>177</v>
       </c>
@@ -5026,7 +5032,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>177</v>
       </c>
@@ -5043,7 +5049,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>177</v>
       </c>
@@ -5060,7 +5066,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -5077,7 +5083,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>177</v>
       </c>
@@ -5094,7 +5100,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>234</v>
       </c>
@@ -5140,7 +5146,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>234</v>
       </c>
@@ -5166,7 +5172,7 @@
         <v>-68.998489000000006</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>234</v>
       </c>
@@ -5192,7 +5198,7 @@
         <v>-69.714607999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>234</v>
       </c>
@@ -5218,7 +5224,7 @@
         <v>-72.543251999999995</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>234</v>
       </c>
@@ -5244,7 +5250,7 @@
         <v>-70.432531999999995</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>234</v>
       </c>
@@ -5270,7 +5276,7 @@
         <v>-73.108534000000006</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>234</v>
       </c>
@@ -5296,7 +5302,7 @@
         <v>-70.967738999999995</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>234</v>
       </c>
@@ -5325,7 +5331,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>234</v>
       </c>
@@ -5351,7 +5357,7 @@
         <v>-73.008763999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>234</v>
       </c>
@@ -5377,7 +5383,7 @@
         <v>-72.588984999999994</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>234</v>
       </c>
@@ -5403,7 +5409,7 @@
         <v>-73.244017999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>-71.727129000000005</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>234</v>
       </c>
@@ -5455,7 +5461,7 @@
         <v>-72.073119000000005</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>234</v>
       </c>
@@ -5481,7 +5487,7 @@
         <v>-70.590025999999995</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>234</v>
       </c>
@@ -5507,7 +5513,7 @@
         <v>-69.456920999999994</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -5533,7 +5539,7 @@
         <v>-71.404539</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>285</v>
       </c>
@@ -5553,7 +5559,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>285</v>
       </c>
@@ -5570,7 +5576,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>285</v>
       </c>
@@ -5587,7 +5593,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>285</v>
       </c>
@@ -5604,7 +5610,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>285</v>
       </c>
@@ -5621,7 +5627,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>285</v>
       </c>
@@ -5638,7 +5644,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>285</v>
       </c>
@@ -5655,7 +5661,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>285</v>
       </c>
@@ -5672,7 +5678,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>285</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>285</v>
       </c>
@@ -5706,7 +5712,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>285</v>
       </c>
@@ -5723,7 +5729,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>285</v>
       </c>
@@ -5740,7 +5746,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>285</v>
       </c>
@@ -5757,7 +5763,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>285</v>
       </c>
@@ -5774,7 +5780,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>285</v>
       </c>
@@ -5791,7 +5797,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>285</v>
       </c>
@@ -5808,7 +5814,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>285</v>
       </c>
@@ -5825,7 +5831,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>285</v>
       </c>
@@ -5842,7 +5848,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>285</v>
       </c>
@@ -5859,7 +5865,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>285</v>
       </c>
@@ -5876,7 +5882,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>285</v>
       </c>
@@ -5893,7 +5899,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>285</v>
       </c>
@@ -5910,7 +5916,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>285</v>
       </c>
@@ -5927,7 +5933,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>285</v>
       </c>
@@ -5944,7 +5950,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>285</v>
       </c>
@@ -5961,7 +5967,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>285</v>
       </c>
@@ -5978,7 +5984,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>285</v>
       </c>
@@ -5998,7 +6004,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>285</v>
       </c>
@@ -6015,7 +6021,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>285</v>
       </c>
@@ -6032,7 +6038,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>285</v>
       </c>
@@ -6049,7 +6055,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>285</v>
       </c>
@@ -6069,7 +6075,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>285</v>
       </c>
@@ -6086,7 +6092,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>285</v>
       </c>
@@ -6103,7 +6109,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>354</v>
       </c>
@@ -6117,7 +6123,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>354</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>354</v>
       </c>
@@ -6145,7 +6151,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>354</v>
       </c>
@@ -6159,7 +6165,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>354</v>
       </c>
@@ -6173,7 +6179,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>354</v>
       </c>
@@ -6187,7 +6193,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>354</v>
       </c>
@@ -6201,7 +6207,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>370</v>
       </c>
@@ -6221,7 +6227,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>370</v>
       </c>
@@ -6241,7 +6247,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>370</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>370</v>
       </c>
@@ -6281,7 +6287,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>370</v>
       </c>
@@ -6301,7 +6307,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>370</v>
       </c>
@@ -6321,7 +6327,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>370</v>
       </c>
@@ -6341,7 +6347,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>370</v>
       </c>
@@ -6361,7 +6367,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>370</v>
       </c>
@@ -6381,7 +6387,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>370</v>
       </c>
@@ -6401,7 +6407,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>370</v>
       </c>
@@ -6421,7 +6427,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>370</v>
       </c>
@@ -6441,7 +6447,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>370</v>
       </c>
@@ -6461,7 +6467,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>370</v>
       </c>
@@ -6481,7 +6487,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>370</v>
       </c>
@@ -6501,7 +6507,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>370</v>
       </c>
@@ -6521,7 +6527,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>370</v>
       </c>
@@ -6541,7 +6547,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -6561,7 +6567,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>370</v>
       </c>
@@ -6581,7 +6587,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>370</v>
       </c>
@@ -6601,7 +6607,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>370</v>
       </c>
@@ -6621,7 +6627,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>370</v>
       </c>
@@ -6641,7 +6647,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>370</v>
       </c>
@@ -6661,7 +6667,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>370</v>
       </c>
@@ -6681,7 +6687,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>370</v>
       </c>
@@ -6701,7 +6707,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>370</v>
       </c>
@@ -6721,7 +6727,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>370</v>
       </c>
@@ -6741,7 +6747,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>370</v>
       </c>
@@ -6761,7 +6767,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>370</v>
       </c>
@@ -6781,7 +6787,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>370</v>
       </c>
@@ -6801,7 +6807,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>370</v>
       </c>
@@ -6821,7 +6827,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>370</v>
       </c>
@@ -6841,7 +6847,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>446</v>
       </c>
@@ -6855,7 +6861,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>446</v>
       </c>
@@ -6869,7 +6875,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>446</v>
       </c>
@@ -6883,7 +6889,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>446</v>
       </c>
@@ -6897,7 +6903,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>446</v>
       </c>
@@ -6911,7 +6917,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>446</v>
       </c>
@@ -6925,7 +6931,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>446</v>
       </c>
@@ -6939,7 +6945,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>446</v>
       </c>
@@ -6953,7 +6959,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>446</v>
       </c>
@@ -6967,7 +6973,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>446</v>
       </c>
@@ -6981,7 +6987,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>446</v>
       </c>
@@ -6995,7 +7001,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>446</v>
       </c>
@@ -7009,7 +7015,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>446</v>
       </c>
@@ -7023,7 +7029,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>446</v>
       </c>
@@ -7037,7 +7043,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>446</v>
       </c>
@@ -7051,7 +7057,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>446</v>
       </c>
@@ -7065,7 +7071,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>446</v>
       </c>
@@ -7079,7 +7085,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>446</v>
       </c>
@@ -7093,7 +7099,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>446</v>
       </c>
@@ -7107,7 +7113,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>446</v>
       </c>
@@ -7121,7 +7127,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>446</v>
       </c>
@@ -7135,7 +7141,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>446</v>
       </c>
@@ -7149,7 +7155,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>446</v>
       </c>
@@ -7163,7 +7169,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>446</v>
       </c>
@@ -7177,7 +7183,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>494</v>
       </c>
@@ -7191,7 +7197,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>494</v>
       </c>
@@ -7205,7 +7211,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>494</v>
       </c>
@@ -7219,7 +7225,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>494</v>
       </c>
@@ -7233,7 +7239,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>494</v>
       </c>
@@ -7247,7 +7253,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>494</v>
       </c>
@@ -7261,7 +7267,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>494</v>
       </c>
@@ -7275,7 +7281,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>494</v>
       </c>
@@ -7289,7 +7295,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>494</v>
       </c>
@@ -7303,7 +7309,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>494</v>
       </c>
@@ -7317,7 +7323,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>494</v>
       </c>
@@ -7331,7 +7337,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>494</v>
       </c>
@@ -7345,7 +7351,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>494</v>
       </c>
@@ -7359,7 +7365,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>494</v>
       </c>
@@ -7373,7 +7379,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>522</v>
       </c>
@@ -7387,7 +7393,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>522</v>
       </c>
@@ -7401,7 +7407,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>522</v>
       </c>
@@ -7415,7 +7421,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>522</v>
       </c>
@@ -7429,7 +7435,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>522</v>
       </c>
@@ -7443,7 +7449,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>522</v>
       </c>
@@ -7457,7 +7463,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>522</v>
       </c>
@@ -7471,7 +7477,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>522</v>
       </c>
@@ -7485,7 +7491,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>522</v>
       </c>
@@ -7499,7 +7505,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>522</v>
       </c>
@@ -7513,7 +7519,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>522</v>
       </c>
@@ -7527,7 +7533,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>522</v>
       </c>
@@ -7541,7 +7547,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>522</v>
       </c>
@@ -7555,7 +7561,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>522</v>
       </c>
@@ -7569,7 +7575,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>522</v>
       </c>
@@ -7583,7 +7589,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>522</v>
       </c>
@@ -7597,7 +7603,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>522</v>
       </c>
@@ -7611,7 +7617,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>522</v>
       </c>
@@ -7625,7 +7631,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>558</v>
       </c>
@@ -7648,7 +7654,7 @@
         <v>-99.151883999999995</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>558</v>
       </c>
@@ -7671,7 +7677,7 @@
         <v>-102.296047</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>558</v>
       </c>
@@ -7694,7 +7700,7 @@
         <v>-115.475579</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>558</v>
       </c>
@@ -7717,7 +7723,7 @@
         <v>-110.30659</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>558</v>
       </c>
@@ -7740,7 +7746,7 @@
         <v>-90.539648999999997</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>558</v>
       </c>
@@ -7766,7 +7772,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>558</v>
       </c>
@@ -7789,7 +7795,7 @@
         <v>-103.72811900000001</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>558</v>
       </c>
@@ -7812,7 +7818,7 @@
         <v>-93.115191999999993</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>558</v>
       </c>
@@ -7835,7 +7841,7 @@
         <v>-106.076307</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>558</v>
       </c>
@@ -7858,7 +7864,7 @@
         <v>-104.670194</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>558</v>
       </c>
@@ -7881,7 +7887,7 @@
         <v>-101.253621</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>558</v>
       </c>
@@ -7904,7 +7910,7 @@
         <v>-99.501063000000002</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>558</v>
       </c>
@@ -7927,7 +7933,7 @@
         <v>-98.737001000000006</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>558</v>
       </c>
@@ -7950,7 +7956,7 @@
         <v>-103.34222200000001</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>558</v>
       </c>
@@ -7973,7 +7979,7 @@
         <v>-99.657317000000006</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>558</v>
       </c>
@@ -7999,7 +8005,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>558</v>
       </c>
@@ -8022,7 +8028,7 @@
         <v>-99.234897000000004</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>558</v>
       </c>
@@ -8045,7 +8051,7 @@
         <v>-104.893799</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>558</v>
       </c>
@@ -8068,7 +8074,7 @@
         <v>-100.310892</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>558</v>
       </c>
@@ -8091,7 +8097,7 @@
         <v>-96.725449999999995</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>558</v>
       </c>
@@ -8114,7 +8120,7 @@
         <v>-98.197495000000004</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>558</v>
       </c>
@@ -8137,7 +8143,7 @@
         <v>-100.389957</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>558</v>
       </c>
@@ -8160,7 +8166,7 @@
         <v>-88.297899000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>558</v>
       </c>
@@ -8183,7 +8189,7 @@
         <v>-100.976958</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>558</v>
       </c>
@@ -8206,7 +8212,7 @@
         <v>-107.393756</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>558</v>
       </c>
@@ -8229,7 +8235,7 @@
         <v>-110.95846400000001</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>558</v>
       </c>
@@ -8252,7 +8258,7 @@
         <v>-92.919415999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>558</v>
       </c>
@@ -8275,7 +8281,7 @@
         <v>-99.151250000000005</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>558</v>
       </c>
@@ -8298,7 +8304,7 @@
         <v>-98.237639999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>558</v>
       </c>
@@ -8324,7 +8330,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>558</v>
       </c>
@@ -8347,7 +8353,7 @@
         <v>-89.624392</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>558</v>
       </c>
@@ -8370,7 +8376,7 @@
         <v>-102.571836</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>628</v>
       </c>
@@ -8387,7 +8393,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>628</v>
       </c>
@@ -8404,7 +8410,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>628</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>628</v>
       </c>
@@ -8438,7 +8444,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>628</v>
       </c>
@@ -8455,7 +8461,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>628</v>
       </c>
@@ -8472,7 +8478,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>628</v>
       </c>
@@ -8489,7 +8495,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>628</v>
       </c>
@@ -8506,7 +8512,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>628</v>
       </c>
@@ -8523,7 +8529,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>628</v>
       </c>
@@ -8540,7 +8546,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>628</v>
       </c>
@@ -8557,7 +8563,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>628</v>
       </c>
@@ -8574,7 +8580,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>628</v>
       </c>
@@ -8591,7 +8597,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>628</v>
       </c>
@@ -8608,7 +8614,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>628</v>
       </c>
@@ -8625,7 +8631,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>628</v>
       </c>
@@ -8642,7 +8648,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>628</v>
       </c>
@@ -8659,7 +8665,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>665</v>
       </c>
@@ -8676,7 +8682,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>665</v>
       </c>
@@ -8693,7 +8699,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>665</v>
       </c>
@@ -8710,7 +8716,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>665</v>
       </c>
@@ -8727,7 +8733,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>665</v>
       </c>
@@ -8744,7 +8750,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>665</v>
       </c>
@@ -8761,7 +8767,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>665</v>
       </c>
@@ -8778,7 +8784,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>665</v>
       </c>
@@ -8795,7 +8801,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>665</v>
       </c>
@@ -8812,7 +8818,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>665</v>
       </c>
@@ -8829,7 +8835,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>665</v>
       </c>
@@ -8846,7 +8852,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>665</v>
       </c>
@@ -8863,7 +8869,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>665</v>
       </c>
@@ -8880,7 +8886,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>693</v>
       </c>
@@ -8897,7 +8903,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>693</v>
       </c>
@@ -8914,7 +8920,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>693</v>
       </c>
@@ -8931,7 +8937,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>693</v>
       </c>
@@ -8948,7 +8954,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>693</v>
       </c>
@@ -8965,7 +8971,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>693</v>
       </c>
@@ -8982,7 +8988,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>693</v>
       </c>
@@ -8999,7 +9005,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>693</v>
       </c>
@@ -9016,7 +9022,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>693</v>
       </c>
@@ -9033,7 +9039,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>693</v>
       </c>
@@ -9050,7 +9056,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>693</v>
       </c>
@@ -9067,7 +9073,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>693</v>
       </c>
@@ -9084,7 +9090,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>693</v>
       </c>
@@ -9101,7 +9107,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>693</v>
       </c>
@@ -9118,7 +9124,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>693</v>
       </c>
@@ -9135,7 +9141,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>693</v>
       </c>
@@ -9152,7 +9158,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>693</v>
       </c>
@@ -9169,7 +9175,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>693</v>
       </c>
@@ -9186,7 +9192,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>730</v>
       </c>
@@ -9200,7 +9206,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>730</v>
       </c>
@@ -9214,7 +9220,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>730</v>
       </c>
@@ -9228,7 +9234,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>730</v>
       </c>
@@ -9242,7 +9248,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>730</v>
       </c>
@@ -9256,7 +9262,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>730</v>
       </c>
@@ -9270,7 +9276,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>730</v>
       </c>
@@ -9284,7 +9290,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>730</v>
       </c>
@@ -9298,7 +9304,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>730</v>
       </c>
@@ -9312,7 +9318,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>730</v>
       </c>
@@ -9326,7 +9332,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>730</v>
       </c>
@@ -9340,7 +9346,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>730</v>
       </c>
@@ -9354,7 +9360,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>730</v>
       </c>
@@ -9368,7 +9374,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>730</v>
       </c>
@@ -9382,7 +9388,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>730</v>
       </c>
@@ -9396,7 +9402,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>730</v>
       </c>
@@ -9410,7 +9416,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>730</v>
       </c>
@@ -9424,7 +9430,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>730</v>
       </c>
@@ -9438,7 +9444,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>730</v>
       </c>
@@ -9452,7 +9458,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>768</v>
       </c>
@@ -9475,7 +9481,7 @@
         <v>-66.879188499999998</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>768</v>
       </c>
@@ -9492,7 +9498,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>768</v>
       </c>
@@ -9515,7 +9521,7 @@
         <v>-67.583427400000005</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>768</v>
       </c>
@@ -9538,7 +9544,7 @@
         <v>-64.616668700000005</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>768</v>
       </c>
@@ -9561,7 +9567,7 @@
         <v>-67.472358700000001</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>768</v>
       </c>
@@ -9584,7 +9590,7 @@
         <v>-67.591133099999993</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>768</v>
       </c>
@@ -9607,7 +9613,7 @@
         <v>-70.207488999999995</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>768</v>
       </c>
@@ -9630,7 +9636,7 @@
         <v>-63.5408592</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>768</v>
       </c>
@@ -9653,7 +9659,7 @@
         <v>-68.007652300000004</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>768</v>
       </c>
@@ -9676,7 +9682,7 @@
         <v>-68.5826797</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>768</v>
       </c>
@@ -9699,7 +9705,7 @@
         <v>-62.049999200000002</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>768</v>
       </c>
@@ -9722,7 +9728,7 @@
         <v>-70.199569699999998</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>768</v>
       </c>
@@ -9745,7 +9751,7 @@
         <v>-67.353813200000005</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>768</v>
       </c>
@@ -9768,7 +9774,7 @@
         <v>-69.357032799999999</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>768</v>
       </c>
@@ -9791,7 +9797,7 @@
         <v>-71.156112699999994</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>768</v>
       </c>
@@ -9814,7 +9820,7 @@
         <v>-66.801551799999999</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>768</v>
       </c>
@@ -9837,7 +9843,7 @@
         <v>-63.183231399999997</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>768</v>
       </c>
@@ -9860,7 +9866,7 @@
         <v>-63.869709</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>768</v>
       </c>
@@ -9883,7 +9889,7 @@
         <v>-69.742057799999998</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>768</v>
       </c>
@@ -9906,7 +9912,7 @@
         <v>-64.182563799999997</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>768</v>
       </c>
@@ -9929,7 +9935,7 @@
         <v>-72.224998499999998</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>768</v>
       </c>
@@ -9952,7 +9958,7 @@
         <v>-70.436943099999993</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>768</v>
       </c>
@@ -9975,7 +9981,7 @@
         <v>-66.954849199999998</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>768</v>
       </c>
@@ -9998,7 +10004,7 @@
         <v>-68.742469799999995</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>768</v>
       </c>
@@ -10022,7 +10028,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L355" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L355">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Peru"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Perú Lat Lon - 2
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="855" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="1830" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="iso3312_latinamerica" sheetId="1" r:id="rId1"/>
@@ -3295,7 +3295,7 @@
   <dimension ref="A1:L355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,7 +3682,7 @@
         <v>-12.0651302</v>
       </c>
       <c r="H13">
-        <v>75.204856899999996</v>
+        <v>-75.204856899999996</v>
       </c>
       <c r="I13" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
fixed overwrite of chilean coordinates
</commit_message>
<xml_diff>
--- a/utils/iso3312_latinamerica.xlsx
+++ b/utils/iso3312_latinamerica.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eica\covid\covid-19_latinoamerica\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanHP\Desktop\GitHub\covid-19_pe\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64450D4A-D255-49AF-8CB0-B5620C2C7927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso3312_latinamerica" sheetId="1" r:id="rId1"/>
@@ -2490,7 +2491,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3290,12 +3291,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,7 +3343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>105</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>157</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>157</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>157</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>157</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>157</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>157</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>157</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>-48.25</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>234</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>238</v>
       </c>
       <c r="G88">
-        <v>-23.55</v>
+        <v>-46.035339</v>
       </c>
       <c r="H88">
         <v>-73.036434999999997</v>
@@ -5308,7 +5308,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>234</v>
       </c>
@@ -5328,13 +5328,13 @@
         <v>242</v>
       </c>
       <c r="G89">
-        <v>-10.25</v>
+        <v>-23.446308999999999</v>
       </c>
       <c r="H89">
         <v>-68.998489000000006</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>234</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>-69.714607999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>234</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>-72.543251999999995</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>234</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>-70.432531999999995</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>234</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>-73.108534000000006</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>234</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>-70.967738999999995</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>234</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>234</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>-73.008763999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>234</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>-72.588984999999994</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>234</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>-73.244017999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>-71.727129000000005</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>234</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>-72.073119000000005</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>234</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>-70.590025999999995</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>234</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>-69.456920999999994</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>-71.404539</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>285</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>285</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>285</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>285</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>285</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>285</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>285</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>285</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>285</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>285</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>285</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>285</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>285</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>285</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>285</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>285</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>285</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>285</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>285</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>285</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>285</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>285</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>285</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>285</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>285</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>285</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>285</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>285</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>285</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>285</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>285</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>285</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>285</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>354</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>354</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>354</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>354</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>354</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>354</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>354</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>370</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>370</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>370</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>370</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>370</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>370</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>370</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>370</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>370</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>370</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>370</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>370</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>370</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>370</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>370</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>370</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>370</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>370</v>
       </c>
@@ -6749,7 +6749,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>370</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>370</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>370</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>370</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>370</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>370</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>370</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>370</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>370</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>370</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>370</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>370</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>370</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>446</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>446</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>446</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>446</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>446</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>446</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>446</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>446</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>446</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>446</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>446</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>446</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>446</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>446</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>446</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>446</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>446</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>446</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>446</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>446</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>446</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>446</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>446</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>446</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>494</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>494</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>494</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>494</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>494</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>494</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>494</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>494</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>494</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>494</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>494</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>494</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>494</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>494</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>522</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>522</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>522</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>522</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>522</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>522</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>522</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>522</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>522</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>522</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>522</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>522</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>522</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>522</v>
       </c>
@@ -7737,7 +7737,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>522</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>522</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>522</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>522</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>558</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>-99.151883999999995</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>558</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>-102.296047</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>558</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>-115.475579</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>558</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>-110.30659</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>558</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>-90.539648999999997</v>
       </c>
     </row>
-    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>558</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>558</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>-103.72811900000001</v>
       </c>
     </row>
-    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>558</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>-93.115191999999993</v>
       </c>
     </row>
-    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>558</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>-106.076307</v>
       </c>
     </row>
-    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>558</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>-104.670194</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>558</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>-101.253621</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>558</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>-99.501063000000002</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>558</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>-98.737001000000006</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>558</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>-103.34222200000001</v>
       </c>
     </row>
-    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>558</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>-99.657317000000006</v>
       </c>
     </row>
-    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>558</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>558</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>-99.234897000000004</v>
       </c>
     </row>
-    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>558</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>-104.893799</v>
       </c>
     </row>
-    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>558</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>-100.310892</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>558</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>-96.725449999999995</v>
       </c>
     </row>
-    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>558</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>-98.197495000000004</v>
       </c>
     </row>
-    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>558</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>-100.389957</v>
       </c>
     </row>
-    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>558</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>-88.297899000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>558</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>-100.976958</v>
       </c>
     </row>
-    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>558</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>-107.393756</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>558</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>-110.95846400000001</v>
       </c>
     </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>558</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>-92.919415999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>558</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>-99.151250000000005</v>
       </c>
     </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>558</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>-98.237639999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>558</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>558</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>-89.624392</v>
       </c>
     </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>558</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>-102.571836</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>628</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>628</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>628</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>628</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>628</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>628</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>628</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>628</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>628</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>628</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>628</v>
       </c>
@@ -8725,7 +8725,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>628</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>628</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>628</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>628</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>628</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>628</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>665</v>
       </c>
@@ -8844,7 +8844,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>665</v>
       </c>
@@ -8861,7 +8861,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>665</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>665</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>665</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>665</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>665</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>665</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>665</v>
       </c>
@@ -8980,7 +8980,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>665</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>665</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>665</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>665</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>693</v>
       </c>
@@ -9065,7 +9065,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>693</v>
       </c>
@@ -9082,7 +9082,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>693</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>693</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>693</v>
       </c>
@@ -9133,7 +9133,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>693</v>
       </c>
@@ -9150,7 +9150,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>693</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>693</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>693</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>693</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>693</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>693</v>
       </c>
@@ -9252,7 +9252,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>693</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>693</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>693</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>693</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>693</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>693</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>730</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>730</v>
       </c>
@@ -9382,7 +9382,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>730</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>730</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>730</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>730</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>730</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>730</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>730</v>
       </c>
@@ -9480,7 +9480,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>730</v>
       </c>
@@ -9494,7 +9494,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>730</v>
       </c>
@@ -9508,7 +9508,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>730</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>730</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>730</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>730</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>730</v>
       </c>
@@ -9578,7 +9578,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>730</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>730</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>730</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>768</v>
       </c>
@@ -9643,7 +9643,7 @@
         <v>-66.879188499999998</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>768</v>
       </c>
@@ -9660,7 +9660,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>768</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>-67.583427400000005</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>768</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>-64.616668700000005</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>768</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>-67.472358700000001</v>
       </c>
     </row>
-    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>768</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>-67.591133099999993</v>
       </c>
     </row>
-    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>768</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>-70.207488999999995</v>
       </c>
     </row>
-    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>768</v>
       </c>
@@ -9798,7 +9798,7 @@
         <v>-63.5408592</v>
       </c>
     </row>
-    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>768</v>
       </c>
@@ -9821,7 +9821,7 @@
         <v>-68.007652300000004</v>
       </c>
     </row>
-    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>768</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>-68.5826797</v>
       </c>
     </row>
-    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>768</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>-62.049999200000002</v>
       </c>
     </row>
-    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>768</v>
       </c>
@@ -9890,7 +9890,7 @@
         <v>-70.199569699999998</v>
       </c>
     </row>
-    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>768</v>
       </c>
@@ -9913,7 +9913,7 @@
         <v>-67.353813200000005</v>
       </c>
     </row>
-    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>768</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>-69.357032799999999</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>768</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>-71.156112699999994</v>
       </c>
     </row>
-    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>768</v>
       </c>
@@ -9982,7 +9982,7 @@
         <v>-66.801551799999999</v>
       </c>
     </row>
-    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>768</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>-63.183231399999997</v>
       </c>
     </row>
-    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>768</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>-63.869709</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>768</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>-69.742057799999998</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>768</v>
       </c>
@@ -10074,7 +10074,7 @@
         <v>-64.182563799999997</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>768</v>
       </c>
@@ -10097,7 +10097,7 @@
         <v>-72.224998499999998</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>768</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>-70.436943099999993</v>
       </c>
     </row>
-    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>768</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>-66.954849199999998</v>
       </c>
     </row>
-    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>768</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>-68.742469799999995</v>
       </c>
     </row>
-    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>768</v>
       </c>
@@ -10190,13 +10190,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L355">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Brazil"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L355" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>